<commit_message>
Update 6 April 2025
</commit_message>
<xml_diff>
--- a/COPD Patient Management Survey.xlsx
+++ b/COPD Patient Management Survey.xlsx
@@ -1632,8 +1632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection sqref="A1:T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3216,25 +3216,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection sqref="A1:T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.109375" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="27.109375" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="28.88671875" hidden="1" customWidth="1"/>
-    <col min="5" max="6" width="0" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="64.21875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="50.5546875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="71.109375" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="46.88671875" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="126.109375" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="36.88671875" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="92.21875" style="4" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="80.44140625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="63.44140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="64.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="50.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="71.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="46.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="126.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="92.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="80.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="63.44140625" customWidth="1"/>
     <col min="16" max="16" width="71" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="68.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="68" bestFit="1" customWidth="1"/>

</xml_diff>